<commit_message>
Add Production Plan Logic
</commit_message>
<xml_diff>
--- a/Code/CoreAPI/API/ExcelUpload/PhysicianSampleForecast/PhysicianSample Forecast.xlsx
+++ b/Code/CoreAPI/API/ExcelUpload/PhysicianSampleForecast/PhysicianSample Forecast.xlsx
@@ -1,25 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B820F3D-7ADD-477B-ADB3-FA17B28DF10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7215" windowHeight="6870"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
   <si>
     <t>CompanyId</t>
   </si>
@@ -39,12 +48,6 @@
     <t>ForecastForMonth</t>
   </si>
   <si>
-    <t>Finish Goods</t>
-  </si>
-  <si>
-    <t>Physician Sample</t>
-  </si>
-  <si>
     <t>ADJULYN</t>
   </si>
   <si>
@@ -63,44 +66,60 @@
     <t>ML</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t>CARMOZYME</t>
+  </si>
+  <si>
+    <t>Product_Name</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
   <si>
     <t>9F5CB879-7B61-4FFD-B8E8-7D05973978E2</t>
   </si>
   <si>
-    <t>Rate</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Product_Name</t>
-  </si>
-  <si>
-    <t>Amount</t>
-  </si>
-  <si>
-    <t>NILI PAIN-S</t>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Depot</t>
+  </si>
+  <si>
+    <t>SLNO</t>
+  </si>
+  <si>
+    <t>Concord</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>MALDA</t>
+  </si>
+  <si>
+    <t>TAMLUK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,11 +156,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,165 +441,334 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.42578125" customWidth="1"/>
-    <col min="9" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2022</v>
+      </c>
+      <c r="D2">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>3500</v>
+      </c>
+      <c r="K2">
+        <v>100</v>
+      </c>
+      <c r="L2" t="s">
         <v>11</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="N2">
+        <v>350000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2022</v>
+      </c>
+      <c r="D3">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>2013</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3">
+        <v>10</v>
+      </c>
+      <c r="N3">
+        <v>20130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2">
+      <c r="C4">
         <v>2022</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2">
-        <v>3500</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>2022</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="D4">
         <v>9</v>
       </c>
-      <c r="G3">
-        <v>2013</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>10</v>
-      </c>
-      <c r="K3">
-        <v>20130</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>2022</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
       <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4">
-        <v>200</v>
-      </c>
-      <c r="H4">
-        <v>10</v>
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
       </c>
       <c r="J4">
+        <v>200</v>
+      </c>
+      <c r="K4">
+        <v>50</v>
+      </c>
+      <c r="L4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4">
         <v>10</v>
       </c>
-      <c r="K4">
+      <c r="N4">
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D13" t="s">
-        <v>14</v>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2022</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>35</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+      <c r="L5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5">
+        <v>100</v>
+      </c>
+      <c r="N5">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>2022</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>2022</v>
+      </c>
+      <c r="D7">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>200</v>
+      </c>
+      <c r="K7">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Chargeable Batch , List Show have been done
</commit_message>
<xml_diff>
--- a/Code/CoreAPI/API/ExcelUpload/PhysicianSampleForecast/PhysicianSample Forecast.xlsx
+++ b/Code/CoreAPI/API/ExcelUpload/PhysicianSampleForecast/PhysicianSample Forecast.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B820F3D-7ADD-477B-ADB3-FA17B28DF10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7215" windowHeight="6870"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
   <si>
     <t>CompanyId</t>
   </si>
@@ -54,9 +53,6 @@
     <t>AMIRID TABLET</t>
   </si>
   <si>
-    <t>BOP</t>
-  </si>
-  <si>
     <t>Pack</t>
   </si>
   <si>
@@ -96,25 +92,22 @@
     <t>Concord</t>
   </si>
   <si>
+    <t>Phoenix</t>
+  </si>
+  <si>
+    <t>MALDA</t>
+  </si>
+  <si>
+    <t>TAMLUK</t>
+  </si>
+  <si>
     <t>IP</t>
-  </si>
-  <si>
-    <t>PS</t>
-  </si>
-  <si>
-    <t>Phoenix</t>
-  </si>
-  <si>
-    <t>MALDA</t>
-  </si>
-  <si>
-    <t>TAMLUK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -441,11 +434,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +450,7 @@
     <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
     <col min="11" max="11" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="7.85546875" bestFit="1" customWidth="1"/>
@@ -468,7 +461,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>4</v>
@@ -477,10 +470,10 @@
         <v>5</v>
       </c>
       <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
         <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -489,30 +482,27 @@
         <v>2</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
       <c r="M1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" t="s">
         <v>15</v>
-      </c>
-      <c r="N1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>2022</v>
@@ -521,17 +511,15 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H2" s="1"/>
       <c r="I2" t="s">
         <v>6</v>
       </c>
@@ -542,21 +530,19 @@
         <v>100</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N2">
-        <v>350000</v>
+        <f>J2*M2</f>
+        <v>35000</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <v>2022</v>
@@ -565,17 +551,15 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="I3" t="s">
         <v>7</v>
       </c>
@@ -586,21 +570,19 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M3">
         <v>10</v>
       </c>
       <c r="N3">
+        <f t="shared" ref="N3:N7" si="0">J3*M3</f>
         <v>20130</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>2022</v>
@@ -609,19 +591,17 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>23</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="H4" s="2"/>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4">
         <v>200</v>
@@ -630,21 +610,19 @@
         <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M4">
         <v>10</v>
       </c>
       <c r="N4">
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C5">
         <v>2022</v>
@@ -653,16 +631,13 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
         <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
       </c>
       <c r="I5" t="s">
         <v>6</v>
@@ -674,21 +649,19 @@
         <v>100</v>
       </c>
       <c r="L5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M5">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="N5">
-        <v>3500</v>
+        <f t="shared" si="0"/>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>2022</v>
@@ -697,16 +670,13 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>23</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -718,21 +688,19 @@
         <v>2</v>
       </c>
       <c r="L6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M6">
         <v>10</v>
       </c>
       <c r="N6">
+        <f t="shared" si="0"/>
         <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>2022</v>
@@ -741,19 +709,16 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" t="s">
         <v>24</v>
       </c>
-      <c r="F7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>23</v>
-      </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J7">
         <v>200</v>
@@ -762,12 +727,13 @@
         <v>50</v>
       </c>
       <c r="L7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M7">
         <v>10</v>
       </c>
       <c r="N7">
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
     </row>

</xml_diff>